<commit_message>
Update cube metadata: Package3
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010026-A-TC-TM-TP.xlsx
+++ b/data/metadata/Informe-01-010026-A-TC-TM-TP.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Informe-05-050314-A-TC-TP" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Informe-01-010026-A-TC-TM-TP" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t xml:space="preserve">Año</t>
   </si>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">xsd:int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mapping-estado-de-la-informacion.xlsx</t>
   </si>
 </sst>
 </file>
@@ -212,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,11 +238,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -289,16 +281,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,31 +307,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="45.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="45.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="57.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="57.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="47.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="58.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="58.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="50.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="38.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,10 +412,10 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -640,20 +625,6 @@
       <c r="S5" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>